<commit_message>
authentication: token, expiration, refreshToken
</commit_message>
<xml_diff>
--- a/comptoir-ws/API.xlsx
+++ b/comptoir-ws/API.xlsx
@@ -333,12 +333,6 @@
     <t>updateEmployee(Employee)</t>
   </si>
   <si>
-    <t>setPassword(EmployeeRef, String)</t>
-  </si>
-  <si>
-    <t>/employee/{employeeId}/password</t>
-  </si>
-  <si>
     <t>register(Registration)</t>
   </si>
   <si>
@@ -370,6 +364,12 @@
   </si>
   <si>
     <t>/employee/{employeeId}/password/{password}</t>
+  </si>
+  <si>
+    <t>refreshAuth(String refreshToken)</t>
+  </si>
+  <si>
+    <t>/auth/refresh/{refreshToken}</t>
   </si>
 </sst>
 </file>
@@ -408,12 +408,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFD966"/>
-        <bgColor rgb="FFFFFF99"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF66CC00"/>
         <bgColor rgb="FF92D050"/>
       </patternFill>
@@ -434,6 +428,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor rgb="FFFFFF99"/>
       </patternFill>
     </fill>
   </fills>
@@ -457,11 +457,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -810,10 +810,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D65"/>
+  <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D61" sqref="D61"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -973,16 +973,16 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="3" t="str">
+      <c r="D13" s="9" t="str">
         <f>"/item/{itemId}/picture/{id}"</f>
         <v>/item/{itemId}/picture/{id}</v>
       </c>
@@ -1009,30 +1009,30 @@
       <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="3" t="s">
+      <c r="C16" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="9" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="9" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1065,44 +1065,44 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="4" t="s">
+      <c r="C21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="3" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" s="3" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1136,16 +1136,16 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D27" s="6" t="str">
+      <c r="D27" s="5" t="str">
         <f>"/sale/{saleId}"</f>
         <v>/sale/{saleId}</v>
       </c>
@@ -1180,398 +1180,398 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="C30" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="D30" s="5" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
+      <c r="A32" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D32" s="5" t="s">
+      <c r="C32" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="4" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
+      <c r="A33" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="C33" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D33" s="4" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
+      <c r="A34" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="C34" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="D34" s="5" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
+      <c r="A35" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C35" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>110</v>
+      <c r="C35" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="6" t="s">
+      <c r="A36" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="C36" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D36" s="6" t="s">
+      <c r="D36" s="5" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="6" t="s">
+      <c r="A38" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B38" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C38" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D38" s="6" t="str">
+      <c r="C38" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" s="5" t="str">
         <f>"/accountingEntry"</f>
         <v>/accountingEntry</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="6" t="s">
+      <c r="A39" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B39" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C39" s="6" t="s">
+      <c r="C39" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D39" s="6" t="str">
+      <c r="D39" s="5" t="str">
         <f>"/accountingEntry/{accountingEntryId}"</f>
         <v>/accountingEntry/{accountingEntryId}</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="B40" s="7" t="s">
+      <c r="A40" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="C40" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>111</v>
-      </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="6" t="s">
+      <c r="A41" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B41" s="6" t="s">
+      <c r="B41" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C41" s="6" t="s">
+      <c r="C41" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D41" s="6" t="str">
+      <c r="D41" s="5" t="str">
         <f>"/accountingEntry/{accountingEntryId}"</f>
         <v>/accountingEntry/{accountingEntryId}</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="6" t="s">
+      <c r="A43" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="B43" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C43" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D43" s="6" t="s">
+      <c r="C43" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" s="5" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="6" t="s">
+      <c r="A44" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B44" s="6" t="s">
+      <c r="B44" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C44" s="6" t="s">
+      <c r="C44" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D44" s="6" t="s">
+      <c r="D44" s="5" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="6" t="s">
+      <c r="A45" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="B45" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C45" s="6" t="s">
+      <c r="C45" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D45" s="6" t="s">
+      <c r="D45" s="5" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="6" t="s">
+      <c r="A46" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B46" s="6" t="s">
+      <c r="B46" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C46" s="6" t="s">
+      <c r="C46" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D46" s="6" t="s">
+      <c r="D46" s="5" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="6" t="s">
+      <c r="A47" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B47" s="6" t="s">
+      <c r="B47" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="C47" s="6" t="s">
+      <c r="C47" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D47" s="6" t="s">
+      <c r="D47" s="5" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="9" t="s">
+      <c r="A49" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="B49" s="9" t="s">
+      <c r="B49" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="C49" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D49" s="9" t="s">
+      <c r="C49" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D49" s="8" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="9" t="s">
+      <c r="A50" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="B50" s="9" t="s">
+      <c r="B50" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="C50" s="9" t="s">
+      <c r="C50" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D50" s="9" t="s">
+      <c r="D50" s="8" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="9" t="s">
+      <c r="A51" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="B51" s="9" t="s">
+      <c r="B51" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="C51" s="9" t="s">
+      <c r="C51" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D51" s="9" t="s">
+      <c r="D51" s="8" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="8" t="s">
+      <c r="A52" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B52" s="8" t="s">
+      <c r="B52" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C52" s="8" t="s">
+      <c r="C52" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D52" s="8" t="s">
+      <c r="D52" s="7" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="8" t="s">
+      <c r="A53" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B53" s="8" t="s">
+      <c r="B53" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="C53" s="8" t="s">
+      <c r="C53" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D53" s="8" t="s">
+      <c r="D53" s="5" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="4" t="s">
+      <c r="A55" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B55" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="C55" s="4" t="s">
+      <c r="C55" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D55" s="4" t="s">
+      <c r="D55" s="3" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="3" t="s">
+      <c r="A56" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B56" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="C56" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D56" s="3" t="s">
+      <c r="C56" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D56" s="9" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="3" t="s">
+      <c r="A57" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B57" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="C57" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D57" s="3" t="s">
+      <c r="C57" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D57" s="9" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="3" t="s">
+      <c r="A58" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="B58" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="C58" s="3" t="s">
+      <c r="C58" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D58" s="3" t="s">
+      <c r="D58" s="9" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="3" t="s">
+      <c r="A59" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B59" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>116</v>
+      <c r="B59" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="C59" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D59" s="9" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B61" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B61" s="2" t="s">
-        <v>114</v>
-      </c>
       <c r="C61" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B63" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B64" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C63" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D63" s="3" t="s">
+      <c r="C64" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D64" s="2" t="s">
         <v>105</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new Sale method: getTotalPayed(Sale)
</commit_message>
<xml_diff>
--- a/comptoir-ws/API.xlsx
+++ b/comptoir-ws/API.xlsx
@@ -15,11 +15,12 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="119">
   <si>
     <t>RETURN TYPE</t>
   </si>
@@ -370,6 +371,12 @@
   </si>
   <si>
     <t>/auth/refresh/{refreshToken}</t>
+  </si>
+  <si>
+    <t>number(,2)</t>
+  </si>
+  <si>
+    <t>getSaleTotalPayed(SaleRef)</t>
   </si>
 </sst>
 </file>
@@ -810,10 +817,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D64"/>
+  <dimension ref="A1:D65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1193,18 +1200,19 @@
         <v>58</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>61</v>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31" s="2" t="str">
+        <f>"/sale/{saleId}/payed"</f>
+        <v>/sale/{saleId}/payed</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1212,70 +1220,69 @@
         <v>59</v>
       </c>
       <c r="B33" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C34" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D34" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B35" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C35" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="D35" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B36" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C35" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D35" s="3" t="s">
+      <c r="C36" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="3" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B37" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C37" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D36" s="4" t="s">
+      <c r="D37" s="4" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D38" s="4" t="str">
-        <f>"/accountingEntry"</f>
-        <v>/accountingEntry</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1283,57 +1290,58 @@
         <v>69</v>
       </c>
       <c r="B39" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="4" t="str">
+        <f>"/accountingEntry"</f>
+        <v>/accountingEntry</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B40" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="C40" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D39" s="4" t="str">
+      <c r="D40" s="4" t="str">
         <f>"/accountingEntry/{accountingEntryId}"</f>
         <v>/accountingEntry/{accountingEntryId}</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="5" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B41" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="C40" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D40" s="5" t="s">
+      <c r="C41" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" s="5" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="4" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B42" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="C42" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D41" s="4" t="str">
+      <c r="D42" s="4" t="str">
         <f>"/accountingEntry/{accountingEntryId}"</f>
         <v>/accountingEntry/{accountingEntryId}</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1341,24 +1349,24 @@
         <v>74</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D45" s="4" t="s">
         <v>78</v>
@@ -1366,13 +1374,13 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>53</v>
+        <v>79</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>55</v>
+        <v>11</v>
       </c>
       <c r="D46" s="4" t="s">
         <v>78</v>
@@ -1380,30 +1388,30 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B48" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C47" s="4" t="s">
+      <c r="C48" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D47" s="4" t="s">
+      <c r="D48" s="4" t="s">
         <v>83</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="B49" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="C49" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D49" s="7" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1411,97 +1419,97 @@
         <v>84</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D51" s="7" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="6" t="s">
+      <c r="A52" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D52" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B52" s="6" t="s">
+      <c r="B53" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="C52" s="6" t="s">
+      <c r="C53" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="D52" s="6" t="s">
+      <c r="D53" s="6" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="4" t="s">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B54" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C53" s="4" t="s">
+      <c r="C54" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D53" s="4" t="s">
+      <c r="D54" s="4" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="9" t="s">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="B55" s="9" t="s">
+      <c r="B56" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="C55" s="9" t="s">
+      <c r="C56" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D55" s="9" t="s">
+      <c r="D56" s="9" t="s">
         <v>96</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="B56" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="C56" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D56" s="8" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="8" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C57" s="8" t="s">
         <v>6</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -1509,41 +1517,41 @@
         <v>100</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="C59" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D59" s="8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="B59" s="8" t="s">
+      <c r="B60" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="C59" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D59" s="8" t="s">
+      <c r="C60" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D60" s="8" t="s">
         <v>114</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -1551,26 +1559,40 @@
         <v>110</v>
       </c>
       <c r="B62" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B63" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="C62" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D62" s="2" t="s">
+      <c r="C63" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D63" s="2" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="B65" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C64" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D64" s="2" t="s">
+      <c r="C65" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D65" s="2" t="s">
         <v>105</v>
       </c>
     </row>

</xml_diff>